<commit_message>
updated but not sure how...
</commit_message>
<xml_diff>
--- a/reanalyzed/sex_marker/SexFindR/visualizations/GWAS_bothRef_genotypes.pval5e-5.ped.xlsx
+++ b/reanalyzed/sex_marker/SexFindR/visualizations/GWAS_bothRef_genotypes.pval5e-5.ped.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miocene/Desktop/git_repos/dissertation/reanalyzed/sex_marker/SexFindR/visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{526AF0D9-3A79-AD41-ABF4-BB57BD57F083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E794FC-FCDD-E442-B829-F623E83B7DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="-20960" windowWidth="34620" windowHeight="20820"/>
+    <workbookView xWindow="140" yWindow="760" windowWidth="34620" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msig_plink_genotypes.ped" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="73">
   <si>
     <t>RX01_1_F_A07_CAGATCTG.sort-n.fixmate-m.sort.markdup-r</t>
   </si>
@@ -233,12 +244,18 @@
   </si>
   <si>
     <t>lg19:11595569</t>
+  </si>
+  <si>
+    <t>male reference genome used</t>
+  </si>
+  <si>
+    <t>female referecne genome used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1422,11 +1439,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1440,6 +1457,14 @@
     <col min="16" max="18" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G2" s="1" t="s">
         <v>66</v>
@@ -2217,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3437,7 +3462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -3543,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -3914,7 +3939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>

</xml_diff>